<commit_message>
work with excel format parameter file and add flat, dark, bias corrections.
</commit_message>
<xml_diff>
--- a/stack_params.xlsx
+++ b/stack_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFB266F-2E06-4790-8980-7E2609060E79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB557B0C-7328-4186-9FD1-139EE9780C89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7940" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21960" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>赤经（ra）</t>
   </si>
@@ -152,7 +152,40 @@
     <t>complex128</t>
   </si>
   <si>
-    <t>/es01/paratera/sce0228/astro/02-26/</t>
+    <t>是否修正：偏置场</t>
+  </si>
+  <si>
+    <t>是否修正：暗场</t>
+  </si>
+  <si>
+    <t>是否修正：平场</t>
+  </si>
+  <si>
+    <t>文件目录：偏置场</t>
+  </si>
+  <si>
+    <t>文件目录：暗场</t>
+  </si>
+  <si>
+    <t>文件目录：平场</t>
+  </si>
+  <si>
+    <t>/es01/paratera/sce0228/astro/general/bias</t>
+  </si>
+  <si>
+    <t>/es01/paratera/sce0228/astro/general/dark</t>
+  </si>
+  <si>
+    <t>/es01/paratera/sce0228/astro/general/flat</t>
+  </si>
+  <si>
+    <t>/home/hao/astro/raw/2022-02-04_20_50_m42</t>
+  </si>
+  <si>
+    <t>进程数设置</t>
+  </si>
+  <si>
+    <t>最大进程数（0代表自动设置）</t>
   </si>
 </sst>
 </file>
@@ -179,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +222,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -224,28 +263,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -526,25 +569,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="2.6328125" customWidth="1"/>
-    <col min="4" max="4" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.81640625" customWidth="1"/>
+    <col min="4" max="4" width="41.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4">
         <v>1</v>
       </c>
@@ -560,234 +603,290 @@
       <c r="E1" s="3">
         <v>5</v>
       </c>
-      <c r="F1" s="3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9">
+        <v>117.181</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>83.818662000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9">
+        <v>31.771999999999998</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>-5.3896790000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="D8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="7">
-        <v>117.181</v>
-      </c>
-      <c r="D3" s="14" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="10">
         <v>0</v>
       </c>
-      <c r="E3" s="11">
-        <v>83.822000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="7">
-        <v>31.771999999999998</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11">
-        <v>-5.391</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="7">
+      <c r="D12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="10">
+        <v>16</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="D8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D15" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="8">
-        <v>16</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>13</v>
+      <c r="D21" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{021A70E6-8F4E-4696-B760-2DF6A5B8B5CF}">
       <formula1>16</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{C0E1F7BC-C680-48DD-B9D4-AEE6B141A13E}">
       <formula1>0</formula1>
       <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22" xr:uid="{ECC3BF82-D661-43F4-90A6-BCEAD41FA7BD}">
+      <formula1>0</formula1>
+      <formula2>1024</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -805,7 +904,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E13 E14 B17 E15</xm:sqref>
+          <xm:sqref>B17 E13:E15 B21:B23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD8923DB-46C5-4634-B959-33317D62F7C5}">
           <x14:formula1>

</xml_diff>

<commit_message>
Try to remove extrema
</commit_message>
<xml_diff>
--- a/stack_params.xlsx
+++ b/stack_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB557B0C-7328-4186-9FD1-139EE9780C89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B311A03-49FF-42CF-9A8F-329AE505DB8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21960" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23060" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,13 +179,13 @@
     <t>/es01/paratera/sce0228/astro/general/flat</t>
   </si>
   <si>
-    <t>/home/hao/astro/raw/2022-02-04_20_50_m42</t>
-  </si>
-  <si>
     <t>进程数设置</t>
   </si>
   <si>
     <t>最大进程数（0代表自动设置）</t>
+  </si>
+  <si>
+    <t>/es01/paratera/sce0228/astro/m42</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -681,7 +681,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>29</v>
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -833,7 +833,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="10">
         <v>48</v>

</xml_diff>

<commit_message>
Fix extrema now works fine
</commit_message>
<xml_diff>
--- a/stack_params.xlsx
+++ b/stack_params.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B311A03-49FF-42CF-9A8F-329AE505DB8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4B5E82-9FA6-4E2D-A731-5DC8055CABCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23060" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1030" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>赤经（ra）</t>
   </si>
@@ -185,7 +185,20 @@
     <t>最大进程数（0代表自动设置）</t>
   </si>
   <si>
-    <t>/es01/paratera/sce0228/astro/m42</t>
+    <t>是否修正：极值</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>修正极值比例</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.00002</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/hao/astro/raw/2022-06-16_22_01_56Z</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -193,13 +206,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -207,8 +220,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -258,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -271,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -286,7 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -569,25 +589,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.81640625" customWidth="1"/>
-    <col min="4" max="4" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" customWidth="1"/>
+    <col min="1" max="1" width="40.9140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.83203125" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>1</v>
       </c>
@@ -604,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -614,7 +634,7 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -628,7 +648,7 @@
         <v>83.818662000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -642,7 +662,7 @@
         <v>-5.3896790000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -650,7 +670,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
@@ -658,13 +678,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -676,12 +696,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>29</v>
@@ -690,7 +710,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
@@ -704,12 +724,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="12">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>41</v>
@@ -718,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>25</v>
       </c>
@@ -732,7 +752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -746,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
@@ -760,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D15" s="7" t="s">
         <v>34</v>
       </c>
@@ -768,13 +788,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -786,7 +806,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>39</v>
       </c>
@@ -800,7 +820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>38</v>
       </c>
@@ -814,7 +834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>43</v>
       </c>
@@ -825,7 +845,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>44</v>
       </c>
@@ -836,10 +856,10 @@
         <v>53</v>
       </c>
       <c r="E22" s="10">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>45</v>
       </c>
@@ -847,11 +867,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>46</v>
       </c>
@@ -859,7 +879,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>47</v>
       </c>
@@ -867,7 +887,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>48</v>
       </c>
@@ -875,7 +895,24 @@
         <v>51</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18" xr:uid="{021A70E6-8F4E-4696-B760-2DF6A5B8B5CF}">
       <formula1>16</formula1>
@@ -904,7 +941,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B17 E13:E15 B21:B23</xm:sqref>
+          <xm:sqref>B17 E13:E15 B21:B23 B29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD8923DB-46C5-4634-B959-33317D62F7C5}">
           <x14:formula1>
@@ -932,12 +969,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -951,7 +988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -966,6 +1003,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for filters
</commit_message>
<xml_diff>
--- a/stack_params.xlsx
+++ b/stack_params.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9410DB86-CC8E-4A21-9FCB-18FDDE623C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341320EA-25EE-44C6-9F2F-6B47C1CB1709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1030" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>赤经（ra）</t>
   </si>
@@ -198,6 +198,10 @@
   </si>
   <si>
     <t>/home/hao/astro/raw/2022-07-07_21_27_18Z</t>
+  </si>
+  <si>
+    <t>保存对齐结果(Save alignment results?)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -591,7 +595,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -792,6 +796,12 @@
         <v>16</v>
       </c>
       <c r="B16" s="5"/>
+      <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
@@ -800,10 +810,6 @@
       <c r="B17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
@@ -812,12 +818,10 @@
       <c r="B18" s="10">
         <v>16</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="D18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -827,9 +831,17 @@
         <v>17</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -840,9 +852,6 @@
       <c r="B21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
@@ -851,11 +860,8 @@
       <c r="B22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
+      <c r="D22" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -864,6 +870,12 @@
       </c>
       <c r="B23" s="11" t="s">
         <v>9</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -920,7 +932,7 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E22" xr:uid="{ECC3BF82-D661-43F4-90A6-BCEAD41FA7BD}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E23" xr:uid="{ECC3BF82-D661-43F4-90A6-BCEAD41FA7BD}">
       <formula1>0</formula1>
       <formula2>1024</formula2>
     </dataValidation>
@@ -940,19 +952,19 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B17 E13:E15 B21:B23 B29</xm:sqref>
+          <xm:sqref>B17 E13:E16 B21:B23 B29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD8923DB-46C5-4634-B959-33317D62F7C5}">
           <x14:formula1>
             <xm:f>Sheet2!$C$1:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E18</xm:sqref>
+          <xm:sqref>E19</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{32E04882-9522-4D48-ADF3-E85548D435D8}">
           <x14:formula1>
             <xm:f>Sheet2!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E19</xm:sqref>
+          <xm:sqref>E20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Improve support for bias, dark and flat
</commit_message>
<xml_diff>
--- a/stack_params.xlsx
+++ b/stack_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DB197C-FFCC-46FF-86D2-EAD0974132CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0092BC9A-5E6D-441D-ACB4-947D85E32E02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4330" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,22 +161,7 @@
     <t>是否修正：平场</t>
   </si>
   <si>
-    <t>文件目录：偏置场</t>
-  </si>
-  <si>
-    <t>文件目录：暗场</t>
-  </si>
-  <si>
     <t>文件目录：平场</t>
-  </si>
-  <si>
-    <t>/es01/paratera/sce0228/astro/general/bias</t>
-  </si>
-  <si>
-    <t>/es01/paratera/sce0228/astro/general/dark</t>
-  </si>
-  <si>
-    <t>/es01/paratera/sce0228/astro/general/flat</t>
   </si>
   <si>
     <t>进程数设置</t>
@@ -205,6 +190,21 @@
   </si>
   <si>
     <t>黑白相机配滤镜必须选True</t>
+  </si>
+  <si>
+    <t>文件：偏置场</t>
+  </si>
+  <si>
+    <t>文件：暗场</t>
+  </si>
+  <si>
+    <t>/astro/294mm-pro/bias-master.fits</t>
+  </si>
+  <si>
+    <t>/astro/294mm-pro/flat/</t>
+  </si>
+  <si>
+    <t>/astro/294mm-pro/dark-master.fits</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -707,7 +707,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>29</v>
@@ -800,13 +800,13 @@
       </c>
       <c r="B16" s="5"/>
       <c r="D16" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -878,7 +878,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E23" s="10">
         <v>0</v>
@@ -890,31 +890,31 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>8</v>
@@ -922,10 +922,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some bugs in multi-channel processing
</commit_message>
<xml_diff>
--- a/stack_params.xlsx
+++ b/stack_params.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0092BC9A-5E6D-441D-ACB4-947D85E32E02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E32B800-B7A3-4300-8C51-5E9DAC726715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8730" yWindow="-110" windowWidth="37480" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>赤经（ra）</t>
   </si>
@@ -198,13 +198,25 @@
     <t>文件：暗场</t>
   </si>
   <si>
-    <t>/astro/294mm-pro/bias-master.fits</t>
-  </si>
-  <si>
-    <t>/astro/294mm-pro/flat/</t>
-  </si>
-  <si>
-    <t>/astro/294mm-pro/dark-master.fits</t>
+    <t>/home/hao/astro/bias-dark-flat/294mm-pro-bin2/bias-master.fits</t>
+  </si>
+  <si>
+    <t>/home/hao/astro/bias-dark-flat/294mm-pro-bin2/dark-master.fits</t>
+  </si>
+  <si>
+    <t>/home/hao/astro/bias-dark-flat</t>
+  </si>
+  <si>
+    <t>HSOLRGB</t>
+  </si>
+  <si>
+    <t>平场通道列表</t>
+  </si>
+  <si>
+    <t>_Bin2_</t>
+  </si>
+  <si>
+    <t>通道名格式（紧邻前缀）</t>
   </si>
 </sst>
 </file>
@@ -598,7 +610,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -735,7 +747,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="12">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>41</v>
@@ -803,7 +815,7 @@
         <v>53</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
         <v>54</v>
@@ -875,7 +887,7 @@
         <v>45</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>48</v>
@@ -895,13 +907,25 @@
       <c r="B25" s="11" t="s">
         <v>57</v>
       </c>
+      <c r="D25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -909,7 +933,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5">

</xml_diff>